<commit_message>
Script to populate tables
</commit_message>
<xml_diff>
--- a/data/Maintenance.xlsx
+++ b/data/Maintenance.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="25" documentId="11_F25DC773A252ABDACC10480A791A596E5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{020EC253-CA71-46EB-90EB-404FBEA81F1B}"/>
   <bookViews>
-    <workbookView xWindow="-24075" yWindow="3720" windowWidth="20130" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32175" yWindow="1350" windowWidth="20130" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>